<commit_message>
Scale by individual PPV
</commit_message>
<xml_diff>
--- a/SEQ02.xlsx
+++ b/SEQ02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pbarbieri\Documents\GitHub\BlastSym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D6AD01-11E4-4A17-B699-718A13A18EEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6CF178-CFA9-43B2-8AA0-0B873DD3D17B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9090" xr2:uid="{2BD00EFF-A5FB-49D2-88BF-24E68AC6C2BC}"/>
   </bookViews>
@@ -797,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D09ABD8-C2C2-42F9-B132-763466854305}">
   <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,6 +839,9 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
+      <c r="F2">
+        <v>61</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -856,6 +859,9 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
+      <c r="F3">
+        <v>61</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -873,6 +879,9 @@
       <c r="E4" t="s">
         <v>11</v>
       </c>
+      <c r="F4">
+        <v>61</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -890,6 +899,9 @@
       <c r="E5" t="s">
         <v>13</v>
       </c>
+      <c r="F5">
+        <v>61</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -907,6 +919,9 @@
       <c r="E6" t="s">
         <v>14</v>
       </c>
+      <c r="F6">
+        <v>61</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -924,6 +939,9 @@
       <c r="E7" t="s">
         <v>7</v>
       </c>
+      <c r="F7">
+        <v>61</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -941,6 +959,9 @@
       <c r="E8" t="s">
         <v>16</v>
       </c>
+      <c r="F8">
+        <v>61</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -958,6 +979,9 @@
       <c r="E9" t="s">
         <v>17</v>
       </c>
+      <c r="F9">
+        <v>61</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -975,6 +999,9 @@
       <c r="E10" t="s">
         <v>18</v>
       </c>
+      <c r="F10">
+        <v>61</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -992,6 +1019,9 @@
       <c r="E11" t="s">
         <v>20</v>
       </c>
+      <c r="F11">
+        <v>61</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1009,6 +1039,9 @@
       <c r="E12" t="s">
         <v>22</v>
       </c>
+      <c r="F12">
+        <v>61</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1026,6 +1059,9 @@
       <c r="E13" t="s">
         <v>24</v>
       </c>
+      <c r="F13">
+        <v>61</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1043,6 +1079,9 @@
       <c r="E14" t="s">
         <v>15</v>
       </c>
+      <c r="F14">
+        <v>61</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1060,6 +1099,9 @@
       <c r="E15" t="s">
         <v>25</v>
       </c>
+      <c r="F15">
+        <v>61</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1077,8 +1119,11 @@
       <c r="E16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1094,8 +1139,11 @@
       <c r="E17" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1111,8 +1159,11 @@
       <c r="E18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1128,8 +1179,11 @@
       <c r="E19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1145,8 +1199,11 @@
       <c r="E20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1162,8 +1219,11 @@
       <c r="E21" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1179,8 +1239,11 @@
       <c r="E22" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1196,8 +1259,11 @@
       <c r="E23" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1213,8 +1279,11 @@
       <c r="E24" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1230,8 +1299,11 @@
       <c r="E25" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1247,8 +1319,11 @@
       <c r="E26" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1264,8 +1339,11 @@
       <c r="E27" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1281,8 +1359,11 @@
       <c r="E28" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1298,8 +1379,11 @@
       <c r="E29" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -1315,8 +1399,11 @@
       <c r="E30" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1332,8 +1419,11 @@
       <c r="E31" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -1349,8 +1439,11 @@
       <c r="E32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1366,8 +1459,11 @@
       <c r="E33" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1383,8 +1479,11 @@
       <c r="E34" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1400,8 +1499,11 @@
       <c r="E35" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1417,8 +1519,11 @@
       <c r="E36" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1434,8 +1539,11 @@
       <c r="E37" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -1451,8 +1559,11 @@
       <c r="E38" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -1468,8 +1579,11 @@
       <c r="E39" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -1485,8 +1599,11 @@
       <c r="E40" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -1502,8 +1619,11 @@
       <c r="E41" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -1519,8 +1639,11 @@
       <c r="E42" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -1536,8 +1659,11 @@
       <c r="E43" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -1553,8 +1679,11 @@
       <c r="E44" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -1570,8 +1699,11 @@
       <c r="E45" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -1587,8 +1719,11 @@
       <c r="E46" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>57</v>
       </c>
@@ -1604,8 +1739,11 @@
       <c r="E47" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -1621,8 +1759,11 @@
       <c r="E48" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -1638,8 +1779,11 @@
       <c r="E49" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -1655,8 +1799,11 @@
       <c r="E50" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -1672,8 +1819,11 @@
       <c r="E51" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1689,8 +1839,11 @@
       <c r="E52" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1706,8 +1859,11 @@
       <c r="E53" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1723,8 +1879,11 @@
       <c r="E54" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1740,8 +1899,11 @@
       <c r="E55" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -1757,8 +1919,11 @@
       <c r="E56" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -1774,8 +1939,11 @@
       <c r="E57" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>60</v>
       </c>
@@ -1791,8 +1959,11 @@
       <c r="E58" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>72</v>
       </c>
@@ -1808,8 +1979,11 @@
       <c r="E59" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>74</v>
       </c>
@@ -1825,8 +1999,11 @@
       <c r="E60" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>76</v>
       </c>
@@ -1842,8 +2019,11 @@
       <c r="E61" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>78</v>
       </c>
@@ -1859,8 +2039,11 @@
       <c r="E62" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>80</v>
       </c>
@@ -1876,8 +2059,11 @@
       <c r="E63" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>81</v>
       </c>
@@ -1893,8 +2079,11 @@
       <c r="E64" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -1910,8 +2099,11 @@
       <c r="E65" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -1927,8 +2119,11 @@
       <c r="E66" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -1944,8 +2139,11 @@
       <c r="E67" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -1961,8 +2159,11 @@
       <c r="E68" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -1978,8 +2179,11 @@
       <c r="E69" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -1995,8 +2199,11 @@
       <c r="E70" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -2012,8 +2219,11 @@
       <c r="E71" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>73</v>
       </c>
@@ -2029,8 +2239,11 @@
       <c r="E72" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>75</v>
       </c>
@@ -2046,8 +2259,11 @@
       <c r="E73" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>77</v>
       </c>
@@ -2063,8 +2279,11 @@
       <c r="E74" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>79</v>
       </c>
@@ -2080,8 +2299,11 @@
       <c r="E75" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -2097,8 +2319,11 @@
       <c r="E76" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -2114,8 +2339,11 @@
       <c r="E77" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -2131,8 +2359,11 @@
       <c r="E78" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -2148,8 +2379,11 @@
       <c r="E79" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>86</v>
       </c>
@@ -2165,8 +2399,11 @@
       <c r="E80" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -2182,8 +2419,11 @@
       <c r="E81" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -2199,8 +2439,11 @@
       <c r="E82" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -2216,8 +2459,11 @@
       <c r="E83" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -2233,8 +2479,11 @@
       <c r="E84" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -2250,8 +2499,11 @@
       <c r="E85" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>92</v>
       </c>
@@ -2267,8 +2519,11 @@
       <c r="E86" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>93</v>
       </c>
@@ -2284,8 +2539,11 @@
       <c r="E87" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>94</v>
       </c>
@@ -2301,8 +2559,11 @@
       <c r="E88" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>95</v>
       </c>
@@ -2318,8 +2579,11 @@
       <c r="E89" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>96</v>
       </c>
@@ -2335,8 +2599,11 @@
       <c r="E90" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>97</v>
       </c>
@@ -2352,8 +2619,11 @@
       <c r="E91" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F91">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>98</v>
       </c>
@@ -2369,8 +2639,11 @@
       <c r="E92" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>99</v>
       </c>
@@ -2386,8 +2659,11 @@
       <c r="E93" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F93">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>100</v>
       </c>
@@ -2403,8 +2679,11 @@
       <c r="E94" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F94">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>101</v>
       </c>
@@ -2420,8 +2699,11 @@
       <c r="E95" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F95">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>102</v>
       </c>
@@ -2437,8 +2719,11 @@
       <c r="E96" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F96">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>103</v>
       </c>
@@ -2454,8 +2739,11 @@
       <c r="E97" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F97">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>104</v>
       </c>
@@ -2471,8 +2759,11 @@
       <c r="E98" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F98">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>105</v>
       </c>
@@ -2488,8 +2779,11 @@
       <c r="E99" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F99">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>106</v>
       </c>
@@ -2505,8 +2799,11 @@
       <c r="E100" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F100">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>107</v>
       </c>
@@ -2522,8 +2819,11 @@
       <c r="E101" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F101">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>108</v>
       </c>
@@ -2539,8 +2839,11 @@
       <c r="E102" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F102">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>109</v>
       </c>
@@ -2556,8 +2859,11 @@
       <c r="E103" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F103">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>110</v>
       </c>
@@ -2573,8 +2879,11 @@
       <c r="E104" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F104">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>111</v>
       </c>
@@ -2590,8 +2899,11 @@
       <c r="E105" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F105">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>112</v>
       </c>
@@ -2607,8 +2919,11 @@
       <c r="E106" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F106">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>113</v>
       </c>
@@ -2624,8 +2939,11 @@
       <c r="E107" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F107">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>114</v>
       </c>
@@ -2641,8 +2959,11 @@
       <c r="E108" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F108">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>115</v>
       </c>
@@ -2658,8 +2979,11 @@
       <c r="E109" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F109">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>116</v>
       </c>
@@ -2675,8 +2999,11 @@
       <c r="E110" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F110">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>117</v>
       </c>
@@ -2692,8 +3019,11 @@
       <c r="E111" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F111">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>118</v>
       </c>
@@ -2709,8 +3039,11 @@
       <c r="E112" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F112">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>119</v>
       </c>
@@ -2726,8 +3059,11 @@
       <c r="E113" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F113">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>120</v>
       </c>
@@ -2743,8 +3079,11 @@
       <c r="E114" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F114">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>121</v>
       </c>
@@ -2760,8 +3099,11 @@
       <c r="E115" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F115">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>122</v>
       </c>
@@ -2777,8 +3119,11 @@
       <c r="E116" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F116">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>123</v>
       </c>
@@ -2794,8 +3139,11 @@
       <c r="E117" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F117">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>124</v>
       </c>
@@ -2811,8 +3159,11 @@
       <c r="E118" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F118">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>125</v>
       </c>
@@ -2828,8 +3179,11 @@
       <c r="E119" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F119">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>126</v>
       </c>
@@ -2845,8 +3199,11 @@
       <c r="E120" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F120">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>127</v>
       </c>
@@ -2862,8 +3219,11 @@
       <c r="E121" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F121">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>128</v>
       </c>
@@ -2879,8 +3239,11 @@
       <c r="E122" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F122">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>129</v>
       </c>
@@ -2896,8 +3259,11 @@
       <c r="E123" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F123">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>130</v>
       </c>
@@ -2913,8 +3279,11 @@
       <c r="E124" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F124">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>131</v>
       </c>
@@ -2930,8 +3299,11 @@
       <c r="E125" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F125">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>132</v>
       </c>
@@ -2947,8 +3319,11 @@
       <c r="E126" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F126">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>133</v>
       </c>
@@ -2964,8 +3339,11 @@
       <c r="E127" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F127">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>134</v>
       </c>
@@ -2981,8 +3359,11 @@
       <c r="E128" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F128">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>135</v>
       </c>
@@ -2998,8 +3379,11 @@
       <c r="E129" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F129">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>136</v>
       </c>
@@ -3015,8 +3399,11 @@
       <c r="E130" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F130">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>137</v>
       </c>
@@ -3031,6 +3418,9 @@
       </c>
       <c r="E131" t="s">
         <v>134</v>
+      </c>
+      <c r="F131">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>